<commit_message>
Update Task metrics value
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -1041,6 +1041,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1056,7 +1057,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,7 +1357,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1365,13 +1365,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="53"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -1379,19 +1379,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="54"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="53"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1399,19 +1399,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="54"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="53"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="53" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1419,19 +1419,19 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="53"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="53" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="55"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
@@ -1626,27 +1626,27 @@
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
@@ -2278,23 +2278,23 @@
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2308,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2354,11 +2354,11 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="31"/>
@@ -2367,11 +2367,11 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="31"/>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="B43" s="15">
         <f>SUM(B2:B42)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="B45" s="47">
         <f>B43/B44*100</f>
-        <v>48.780487804878049</v>
+        <v>53.658536585365859</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -3118,7 +3118,7 @@
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="52">
         <v>0</v>
       </c>
       <c r="C6" s="19"/>
@@ -3129,7 +3129,7 @@
       <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="52">
         <v>0</v>
       </c>
       <c r="C7" s="19"/>
@@ -3140,7 +3140,7 @@
       <c r="A8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="52">
         <v>0</v>
       </c>
       <c r="C8" s="19"/>
@@ -3151,7 +3151,7 @@
       <c r="A9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="52">
         <v>0</v>
       </c>
       <c r="C9" s="19"/>
@@ -3161,7 +3161,7 @@
       <c r="A10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="52">
         <v>0</v>
       </c>
       <c r="C10" s="19"/>
@@ -3171,7 +3171,7 @@
       <c r="A11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="52">
         <v>0</v>
       </c>
       <c r="C11" s="19"/>
@@ -3181,7 +3181,7 @@
       <c r="A12" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="52">
         <v>0</v>
       </c>
       <c r="C12" s="19"/>
@@ -3191,7 +3191,7 @@
       <c r="A13" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="57">
+      <c r="B13" s="52">
         <v>0</v>
       </c>
       <c r="C13" s="37"/>
@@ -3201,7 +3201,7 @@
       <c r="A14" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="57">
+      <c r="B14" s="52">
         <v>0</v>
       </c>
       <c r="C14" s="37"/>
@@ -3211,7 +3211,7 @@
       <c r="A15" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="57">
+      <c r="B15" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       <c r="A16" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       <c r="A17" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="57">
+      <c r="B17" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3235,7 +3235,7 @@
       <c r="A18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3243,7 +3243,7 @@
       <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="57">
+      <c r="B19" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3251,7 +3251,7 @@
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="57">
+      <c r="B20" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       <c r="A21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="57">
+      <c r="B21" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       <c r="A22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="57">
+      <c r="B22" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3602,7 +3602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update bug metrics with new bugs issued on GITLAB. Updated task metrics completion value.
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
   <si>
     <t>Task</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Slides for PM Review</t>
   </si>
   <si>
-    <t>Bootstrap function and Update SDs  is pushed over to iterartion 3</t>
-  </si>
-  <si>
     <t>Prepare Testcase for delete data function</t>
   </si>
   <si>
@@ -347,12 +344,6 @@
     <t>Debug Bootstrap</t>
   </si>
   <si>
-    <t>Integrate all functions</t>
-  </si>
-  <si>
-    <t>Deploy all functions</t>
-  </si>
-  <si>
     <t>Basic App Report JSON</t>
   </si>
   <si>
@@ -362,9 +353,6 @@
     <t>Test Basic App Usage</t>
   </si>
   <si>
-    <t>Test CRUD Location</t>
-  </si>
-  <si>
     <t>Peer Sharing</t>
   </si>
   <si>
@@ -480,6 +468,18 @@
   </si>
   <si>
     <t>Go ahead with planned schedule without any changes to buffer timing.</t>
+  </si>
+  <si>
+    <t>Debug Heatmap</t>
+  </si>
+  <si>
+    <t>Deploy to OpenShift</t>
+  </si>
+  <si>
+    <t>Bootstrap function pushed over to iterartion 3</t>
+  </si>
+  <si>
+    <t>Test Delete Location</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C13" s="57"/>
       <c r="D13" s="57"/>
@@ -2032,7 +2032,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2156,7 +2156,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B20" s="13">
         <f>SUM(B2:B19)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B22" s="36">
         <f>B20/B21*100</f>
-        <v>66.666666666666657</v>
+        <v>72.222222222222214</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
@@ -2279,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -2306,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4">
         <v>0</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="51" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="4">
         <v>0</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="51" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="41">
         <v>1</v>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="41">
         <v>1</v>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="41">
         <v>1</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="41">
         <v>1</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="41">
         <v>0</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="41">
         <v>0</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" s="45">
         <v>0</v>
@@ -2665,28 +2665,28 @@
       <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="50" t="s">
-        <v>79</v>
+      <c r="A33" s="39" t="s">
+        <v>113</v>
       </c>
       <c r="B33" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="50" t="s">
-        <v>81</v>
+      <c r="A34" s="39" t="s">
+        <v>75</v>
       </c>
       <c r="B34" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="50" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B35" s="45">
         <v>0</v>
@@ -2696,37 +2696,37 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="41">
-        <v>0</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B36" s="45">
+        <v>0</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="50" t="s">
-        <v>73</v>
+      <c r="A37" s="39" t="s">
+        <v>93</v>
       </c>
       <c r="B37" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="50" t="s">
-        <v>80</v>
+      <c r="A38" s="39" t="s">
+        <v>114</v>
       </c>
       <c r="B38" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="50" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B39" s="41">
         <v>0</v>
@@ -2735,7 +2735,7 @@
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="50" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="41">
@@ -2746,72 +2746,76 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="49" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B41" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="49" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="B42" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="15">
-        <f>SUM(B2:B42)</f>
-        <v>22</v>
+      <c r="A43" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="41">
+        <v>1</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="16">
-        <f>COUNT(B2:B42)</f>
-        <v>41</v>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="15">
+        <f>SUM(B2:B43)</f>
+        <v>29</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="47">
-        <f>B43/B44*100</f>
-        <v>53.658536585365859</v>
+      <c r="A45" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="16">
+        <f>COUNT(B2:B43)</f>
+        <v>42</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="48"/>
+      <c r="A46" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="47">
+        <f>B44/B45*100</f>
+        <v>69.047619047619051</v>
+      </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
+    <row r="47" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="48"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -3005,6 +3009,9 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
@@ -3041,6 +3048,9 @@
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3072,7 +3082,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3083,7 +3093,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3094,7 +3104,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3105,7 +3115,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -3116,7 +3126,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B6" s="52">
         <v>0</v>
@@ -3127,7 +3137,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B7" s="52">
         <v>0</v>
@@ -3138,7 +3148,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B8" s="52">
         <v>0</v>
@@ -3149,7 +3159,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B9" s="52">
         <v>0</v>
@@ -3159,7 +3169,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B10" s="52">
         <v>0</v>
@@ -3169,7 +3179,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B11" s="52">
         <v>0</v>
@@ -3179,7 +3189,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B12" s="52">
         <v>0</v>
@@ -3189,7 +3199,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="39" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B13" s="52">
         <v>0</v>
@@ -3199,7 +3209,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B14" s="52">
         <v>0</v>
@@ -3209,7 +3219,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="46" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B15" s="52">
         <v>0</v>
@@ -3217,7 +3227,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B16" s="52">
         <v>0</v>
@@ -3225,7 +3235,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B17" s="52">
         <v>0</v>
@@ -3233,7 +3243,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B18" s="52">
         <v>0</v>
@@ -3241,7 +3251,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B19" s="52">
         <v>0</v>
@@ -3257,7 +3267,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B21" s="52">
         <v>0</v>
@@ -3265,7 +3275,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B22" s="52">
         <v>0</v>
@@ -3273,7 +3283,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -3416,7 +3426,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3426,7 +3436,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3436,7 +3446,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3446,7 +3456,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3456,7 +3466,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3466,7 +3476,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3486,7 +3496,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3625,7 +3635,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3636,7 +3646,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3647,7 +3657,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3669,7 +3679,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Update Task Metrics with mitigation plan while doing PM Handover
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
   <si>
     <t>Task</t>
   </si>
@@ -359,12 +359,6 @@
     <t>Debug Login</t>
   </si>
   <si>
-    <t>Debug in openshift</t>
-  </si>
-  <si>
-    <t>Debug CRUD</t>
-  </si>
-  <si>
     <t>Regression Testing</t>
   </si>
   <si>
@@ -480,6 +474,18 @@
   </si>
   <si>
     <t>Test Delete Location</t>
+  </si>
+  <si>
+    <t>Debug Delete Location</t>
+  </si>
+  <si>
+    <t>Debug after deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Pass basic app (logic,UI,JSON,Testing)
+2)Test &amp; Debug Delete Location
+3)Debug Bootstrap
+</t>
   </si>
 </sst>
 </file>
@@ -518,7 +524,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,25 +563,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,19 +689,6 @@
         <color indexed="64"/>
       </left>
       <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -936,11 +911,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -961,44 +945,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1015,7 +999,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1028,35 +1012,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,7 +1343,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="48" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1365,13 +1351,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="54"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="48" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -1379,19 +1365,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="54"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1399,19 +1385,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="54"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="48" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1419,19 +1405,19 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="54"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="48" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -1439,7 +1425,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="56"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
@@ -1626,27 +1612,27 @@
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="B13" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
@@ -2278,23 +2264,23 @@
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="B23" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2308,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2380,11 +2366,11 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="39" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="31"/>
@@ -2535,27 +2521,27 @@
       <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="39" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="55" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="4">
@@ -2565,8 +2551,8 @@
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="51" t="s">
-        <v>116</v>
+      <c r="A23" s="55" t="s">
+        <v>114</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -2625,7 +2611,7 @@
       <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="55" t="s">
         <v>69</v>
       </c>
       <c r="B29" s="41">
@@ -2635,7 +2621,7 @@
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="55" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="41">
@@ -2645,30 +2631,30 @@
       <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="45">
+      <c r="B31" s="44">
         <v>0</v>
       </c>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="45">
-        <v>0</v>
+      <c r="B32" s="44">
+        <v>1</v>
       </c>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="B33" s="45">
+        <v>111</v>
+      </c>
+      <c r="B33" s="44">
         <v>1</v>
       </c>
       <c r="C33" s="38"/>
@@ -2678,27 +2664,27 @@
       <c r="A34" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="45">
+      <c r="B34" s="44">
         <v>1</v>
       </c>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="45">
+      <c r="A35" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="44">
         <v>0</v>
       </c>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="44">
         <v>0</v>
       </c>
       <c r="C36" s="38"/>
@@ -2706,7 +2692,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B37" s="41">
         <v>1</v>
@@ -2716,7 +2702,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B38" s="41">
         <v>1</v>
@@ -2725,27 +2711,27 @@
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="50" t="s">
-        <v>76</v>
+      <c r="A39" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="B39" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="50" t="s">
-        <v>78</v>
+      <c r="A40" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="B40" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="39" t="s">
         <v>74</v>
       </c>
       <c r="B41" s="41">
@@ -2755,7 +2741,7 @@
       <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="41">
@@ -2765,8 +2751,8 @@
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="49" t="s">
-        <v>79</v>
+      <c r="A43" s="39" t="s">
+        <v>77</v>
       </c>
       <c r="B43" s="41">
         <v>1</v>
@@ -2780,7 +2766,7 @@
       </c>
       <c r="B44" s="15">
         <f>SUM(B2:B43)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -2800,20 +2786,22 @@
       <c r="A46" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="47">
+      <c r="B46" s="46">
         <f>B44/B45*100</f>
-        <v>69.047619047619051</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" ht="88" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+      <c r="B47" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
     </row>
     <row r="48" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
@@ -3053,6 +3041,9 @@
       <c r="A93" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B47:D47"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3061,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3082,7 +3073,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3093,7 +3084,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3104,7 +3095,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3115,7 +3106,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -3126,9 +3117,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="52">
+        <v>87</v>
+      </c>
+      <c r="B6" s="47">
         <v>0</v>
       </c>
       <c r="C6" s="19"/>
@@ -3137,9 +3128,9 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="52">
+        <v>80</v>
+      </c>
+      <c r="B7" s="47">
         <v>0</v>
       </c>
       <c r="C7" s="19"/>
@@ -3148,9 +3139,9 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="52">
+        <v>81</v>
+      </c>
+      <c r="B8" s="47">
         <v>0</v>
       </c>
       <c r="C8" s="19"/>
@@ -3159,9 +3150,9 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="52">
+        <v>86</v>
+      </c>
+      <c r="B9" s="47">
         <v>0</v>
       </c>
       <c r="C9" s="19"/>
@@ -3169,9 +3160,9 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="52">
+        <v>88</v>
+      </c>
+      <c r="B10" s="47">
         <v>0</v>
       </c>
       <c r="C10" s="19"/>
@@ -3179,9 +3170,9 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="52">
+        <v>82</v>
+      </c>
+      <c r="B11" s="47">
         <v>0</v>
       </c>
       <c r="C11" s="19"/>
@@ -3189,9 +3180,9 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="52">
+        <v>92</v>
+      </c>
+      <c r="B12" s="47">
         <v>0</v>
       </c>
       <c r="C12" s="19"/>
@@ -3199,9 +3190,9 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="52">
+        <v>95</v>
+      </c>
+      <c r="B13" s="47">
         <v>0</v>
       </c>
       <c r="C13" s="37"/>
@@ -3209,51 +3200,51 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="52">
+        <v>98</v>
+      </c>
+      <c r="B14" s="47">
         <v>0</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="52">
+      <c r="A15" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="52">
+        <v>93</v>
+      </c>
+      <c r="B16" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="52">
+        <v>83</v>
+      </c>
+      <c r="B17" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="52">
+        <v>89</v>
+      </c>
+      <c r="B18" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="52">
+        <v>90</v>
+      </c>
+      <c r="B19" s="47">
         <v>0</v>
       </c>
     </row>
@@ -3261,29 +3252,29 @@
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="52">
+        <v>91</v>
+      </c>
+      <c r="B21" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="52">
+        <v>96</v>
+      </c>
+      <c r="B22" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -3426,7 +3417,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3436,7 +3427,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3446,7 +3437,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3456,7 +3447,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3466,7 +3457,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3476,7 +3467,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3496,7 +3487,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3635,7 +3626,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3646,7 +3637,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3657,7 +3648,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3679,7 +3670,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Continue(update mitigation plan as previous plan not clear)
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -482,10 +482,10 @@
     <t>Debug after deployment</t>
   </si>
   <si>
-    <t xml:space="preserve">1) Pass basic app (logic,UI,JSON,Testing)
+    <t>1) basic app (logic,UI,JSON,Testing)
 2)Test &amp; Debug Delete Location
 3)Debug Bootstrap
-</t>
+Pass all this to Next Iter</t>
   </si>
 </sst>
 </file>
@@ -2294,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated the Metrics for Supervisor Meeting 9
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
   <si>
     <t>Task</t>
   </si>
@@ -365,12 +365,6 @@
     <t>Update next Iteration</t>
   </si>
   <si>
-    <t>Test case for Smartphone usage heatmap</t>
-  </si>
-  <si>
-    <t>Testcase top-K</t>
-  </si>
-  <si>
     <t>Update Diagrams</t>
   </si>
   <si>
@@ -380,21 +374,9 @@
     <t>Supervisor Meeting</t>
   </si>
   <si>
-    <t>Test case for Smartphone overuse report</t>
-  </si>
-  <si>
-    <t>Top-K Usage Report Logic</t>
-  </si>
-  <si>
-    <t>Top-K Usage Report UI</t>
-  </si>
-  <si>
     <t>Social Activeness Report UI</t>
   </si>
   <si>
-    <t>Top-K Usage Report JSON</t>
-  </si>
-  <si>
     <t>Social Activeness Report JSON</t>
   </si>
   <si>
@@ -417,12 +399,6 @@
   </si>
   <si>
     <t>Smartphone overuse report UI</t>
-  </si>
-  <si>
-    <t>Test on Openshift</t>
-  </si>
-  <si>
-    <t>Debug on openshift</t>
   </si>
   <si>
     <t>Smartphone overuse report JSON</t>
@@ -486,13 +462,77 @@
 2)Test &amp; Debug Delete Location
 3)Debug Bootstrap
 Pass all this to Next Iter</t>
+  </si>
+  <si>
+    <t>Update Bug Metrics</t>
+  </si>
+  <si>
+    <t>Bootstrap Diagram</t>
+  </si>
+  <si>
+    <t>Develop Top-K students Most Apps usage (App Cat)</t>
+  </si>
+  <si>
+    <t>Develop Top-K schools Most Apps usage (App Cat)</t>
+  </si>
+  <si>
+    <t>Deploy application to OpenShift (Overuse + Basic App)</t>
+  </si>
+  <si>
+    <t>Deploy application to OpenShift (Top-K + Activeness)</t>
+  </si>
+  <si>
+    <t>Debugging Overuse</t>
+  </si>
+  <si>
+    <t>Debugging Basic App</t>
+  </si>
+  <si>
+    <t>Building of Test Cases
+Top-K</t>
+  </si>
+  <si>
+    <t>Building of Test Cases (Smartphone Overuse Report)</t>
+  </si>
+  <si>
+    <t>Building of Test Cases (Social Activeness)</t>
+  </si>
+  <si>
+    <t>Building of Test Cases (Basic App)</t>
+  </si>
+  <si>
+    <t>Testing on OpenShift (Overuse)</t>
+  </si>
+  <si>
+    <t>Testing on OpenShift (Basic App)</t>
+  </si>
+  <si>
+    <t>Friday Meeting</t>
+  </si>
+  <si>
+    <t>Friday Meeting (PM handover)</t>
+  </si>
+  <si>
+    <t>Pre-Supervisor Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparation of slides for Supervisor Meeting (Week 9) </t>
+  </si>
+  <si>
+    <t>Debug Basic App Usage</t>
+  </si>
+  <si>
+    <t>Debug Smartphone Overuse Report</t>
+  </si>
+  <si>
+    <t>Test Smartphone Overuse Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,6 +562,13 @@
       <sz val="9"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -568,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -920,11 +967,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1021,6 +1092,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1042,7 +1114,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,12 +1408,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="98.08984375" customWidth="1"/>
+    <col min="2" max="2" width="98.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -1342,95 +1421,95 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+    <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49"/>
+    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="50"/>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="49"/>
+    <row r="6" spans="1:2" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
+    <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="49"/>
+    <row r="9" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="49"/>
+    <row r="12" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:2" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="49" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="51"/>
+    <row r="14" spans="1:2" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="52"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
@@ -1451,18 +1530,18 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="94.26953125" customWidth="1"/>
-    <col min="6" max="6" width="32.7265625" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" customWidth="1"/>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="94.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1552,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1564,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1497,7 +1576,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1509,7 +1588,7 @@
       <c r="E4" s="31"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1521,7 +1600,7 @@
       <c r="E5" s="32"/>
       <c r="F5" s="30"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1533,7 +1612,7 @@
       <c r="E6" s="32"/>
       <c r="F6" s="30"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1624,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="30"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1636,7 @@
       <c r="E8" s="32"/>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1648,7 @@
       <c r="E9" s="32"/>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1661,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="30"/>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1595,7 +1674,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -1608,35 +1687,35 @@
       <c r="E12" s="33"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+      <c r="B13" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -1644,7 +1723,7 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -1652,7 +1731,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1660,7 +1739,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="30"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -1668,7 +1747,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="19"/>
@@ -1676,332 +1755,332 @@
       <c r="E20" s="19"/>
       <c r="F20" s="30"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="6"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
     </row>
   </sheetData>
@@ -2021,13 +2100,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2116,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -2049,7 +2128,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -2061,7 +2140,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2073,7 +2152,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -2085,7 +2164,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2097,7 +2176,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -2107,7 +2186,7 @@
       <c r="C7" s="19"/>
       <c r="D7" s="31"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2117,7 +2196,7 @@
       <c r="C8" s="19"/>
       <c r="D8" s="31"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2127,7 +2206,7 @@
       <c r="C9" s="19"/>
       <c r="D9" s="31"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2137,7 +2216,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -2147,7 +2226,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2157,7 +2236,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -2167,7 +2246,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -2177,7 +2256,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2187,7 +2266,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -2197,7 +2276,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -2207,7 +2286,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -2217,7 +2296,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -2227,7 +2306,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>11</v>
       </c>
@@ -2238,7 +2317,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
@@ -2249,7 +2328,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>13</v>
       </c>
@@ -2260,27 +2339,27 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2294,16 +2373,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:D47"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.36328125" customWidth="1"/>
+    <col min="1" max="1" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2392,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -2326,7 +2405,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -2339,7 +2418,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
@@ -2352,7 +2431,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
@@ -2365,7 +2444,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>43</v>
       </c>
@@ -2378,7 +2457,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -2391,7 +2470,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -2404,7 +2483,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
@@ -2417,7 +2496,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -2430,7 +2509,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -2440,7 +2519,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2450,7 +2529,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>54</v>
       </c>
@@ -2460,7 +2539,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -2470,7 +2549,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -2480,7 +2559,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -2490,7 +2569,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2500,7 +2579,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2510,7 +2589,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>62</v>
       </c>
@@ -2520,7 +2599,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
         <v>61</v>
       </c>
@@ -2530,7 +2609,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
         <v>63</v>
       </c>
@@ -2540,8 +2619,8 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="55" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="4">
@@ -2550,9 +2629,9 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="55" t="s">
-        <v>114</v>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>106</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -2560,7 +2639,7 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>64</v>
       </c>
@@ -2570,7 +2649,7 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="39" t="s">
         <v>65</v>
       </c>
@@ -2580,7 +2659,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
         <v>67</v>
       </c>
@@ -2590,7 +2669,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>68</v>
       </c>
@@ -2600,7 +2679,7 @@
       <c r="C27" s="19"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
         <v>66</v>
       </c>
@@ -2610,8 +2689,8 @@
       <c r="C28" s="19"/>
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="55" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
         <v>69</v>
       </c>
       <c r="B29" s="41">
@@ -2620,8 +2699,8 @@
       <c r="C29" s="19"/>
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="55" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="41">
@@ -2630,8 +2709,8 @@
       <c r="C30" s="19"/>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="55" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="48" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="44">
@@ -2640,7 +2719,7 @@
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="39" t="s">
         <v>46</v>
       </c>
@@ -2650,9 +2729,9 @@
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B33" s="44">
         <v>1</v>
@@ -2660,7 +2739,7 @@
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
         <v>75</v>
       </c>
@@ -2670,9 +2749,9 @@
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="55" t="s">
-        <v>115</v>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>107</v>
       </c>
       <c r="B35" s="44">
         <v>0</v>
@@ -2680,8 +2759,8 @@
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="55" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="48" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="44">
@@ -2690,9 +2769,9 @@
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B37" s="41">
         <v>1</v>
@@ -2700,9 +2779,9 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B38" s="41">
         <v>1</v>
@@ -2710,9 +2789,9 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="39" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B39" s="41">
         <v>1</v>
@@ -2720,7 +2799,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
         <v>76</v>
       </c>
@@ -2730,7 +2809,7 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
         <v>74</v>
       </c>
@@ -2740,7 +2819,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>9</v>
       </c>
@@ -2750,7 +2829,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
         <v>77</v>
       </c>
@@ -2760,7 +2839,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
@@ -2771,7 +2850,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>12</v>
       </c>
@@ -2782,7 +2861,7 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="43" t="s">
         <v>13</v>
       </c>
@@ -2793,251 +2872,251 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="88" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" ht="87.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
     </row>
   </sheetData>
@@ -3050,19 +3129,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" customWidth="1"/>
+    <col min="1" max="1" width="79.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -3071,325 +3151,525 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="57">
         <v>0</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="47">
+        <v>1</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="47">
+        <v>0</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="47">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="47">
+        <v>0</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="47">
+        <v>1</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="47">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="47">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="47">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="47">
+        <v>0</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="47">
+        <v>0</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="47">
+        <v>0</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="47">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="47">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="47">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="47">
+        <v>0</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="47">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="47">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="47">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="47">
+        <v>0</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="31"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="47">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="47">
+        <v>0</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="31"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="47">
+        <v>0</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="31"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="47">
+        <v>0</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="31"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="47">
+        <v>0</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="31"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="47">
+        <v>0</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="47">
+        <v>0</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="B34" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="47">
-        <v>0</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="47">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="47">
-        <v>0</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="47">
-        <v>0</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="47">
-        <v>0</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="31"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="47">
-        <v>0</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="31"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="47">
-        <v>0</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="31"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="47">
-        <v>0</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="47">
-        <v>0</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="10" t="s">
+      <c r="B39" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="13">
-        <f>SUM(B2:B23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="14" t="s">
+      <c r="B44" s="13">
+        <f>SUM(B2:B43)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="15">
-        <f>COUNT(B2:B23)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="17" t="s">
+      <c r="B45" s="15">
+        <f>COUNT(B2:B43)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="36">
-        <f>B24/B25*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="B46" s="36">
+        <f>B44/B45*100</f>
+        <v>7.1428571428571423</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="37"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="37"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
+      <c r="B47" s="37"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="37"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3401,13 +3681,13 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="81.90625" customWidth="1"/>
+    <col min="1" max="1" width="81.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3415,9 +3695,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3425,9 +3705,9 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3435,9 +3715,9 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3445,9 +3725,9 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3455,9 +3735,9 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3465,9 +3745,9 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3475,7 +3755,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3485,9 +3765,9 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3495,73 +3775,73 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -3570,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>12</v>
       </c>
@@ -3579,7 +3859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>13</v>
       </c>
@@ -3588,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>2</v>
       </c>
@@ -3607,13 +3887,13 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.26953125" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3624,9 +3904,9 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3635,9 +3915,9 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3646,9 +3926,9 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3657,7 +3937,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -3668,9 +3948,9 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3679,95 +3959,95 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -3776,7 +4056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>12</v>
       </c>
@@ -3785,7 +4065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>13</v>
       </c>
@@ -3794,18 +4074,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="37"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>

</xml_diff>

<commit_message>
Updated bootstrap diagram, updated task metrics and updated bug metrics, updated with Top-K test cases
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="138">
   <si>
     <t>Task</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Social Activeness Report JSON</t>
   </si>
   <si>
-    <t>Debug Smartphone Usage Heatmap</t>
-  </si>
-  <si>
     <t>Debug Top-K</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
   </si>
   <si>
     <t>Test TOP-K</t>
-  </si>
-  <si>
-    <t>Test Smartphone Usage Heatmap</t>
   </si>
   <si>
     <t>Smartphone overuse report UI</t>
@@ -479,9 +473,6 @@
     <t>Deploy application to OpenShift (Overuse + Basic App)</t>
   </si>
   <si>
-    <t>Deploy application to OpenShift (Top-K + Activeness)</t>
-  </si>
-  <si>
     <t>Debugging Overuse</t>
   </si>
   <si>
@@ -526,6 +517,36 @@
   </si>
   <si>
     <t>Test Smartphone Overuse Report</t>
+  </si>
+  <si>
+    <t>Basic App Report Function1</t>
+  </si>
+  <si>
+    <t>Basic App Report Function2</t>
+  </si>
+  <si>
+    <t>Basic App Report Function3</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Deploy application to OpenShift (Top-K)</t>
+  </si>
+  <si>
+    <t>Test Basic App Usage (Openshift)</t>
+  </si>
+  <si>
+    <t>Test Delete Location (Openshift)</t>
+  </si>
+  <si>
+    <t>Debug Delete Location (Openshift)</t>
+  </si>
+  <si>
+    <t>Debug Bootstrap (Openshift)</t>
+  </si>
+  <si>
+    <t>Preparation of Material for supervisor Meeting</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1089,10 +1110,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1113,14 +1141,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1422,7 +1442,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1430,13 +1450,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="52" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -1444,19 +1464,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1464,19 +1484,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="52" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1484,19 +1504,19 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="52" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -1504,7 +1524,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
@@ -1691,27 +1711,27 @@
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="B13" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
@@ -2097,7 +2117,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,23 +2363,23 @@
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
+      <c r="B23" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2373,7 +2393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:A36"/>
     </sheetView>
   </sheetViews>
@@ -2620,7 +2640,7 @@
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="47" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="4">
@@ -2630,8 +2650,8 @@
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
-        <v>106</v>
+      <c r="A23" s="47" t="s">
+        <v>104</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -2690,7 +2710,7 @@
       <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="47" t="s">
         <v>69</v>
       </c>
       <c r="B29" s="41">
@@ -2700,7 +2720,7 @@
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="47" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="41">
@@ -2710,7 +2730,7 @@
       <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="47" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="44">
@@ -2731,7 +2751,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="44">
         <v>1</v>
@@ -2750,8 +2770,8 @@
       <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
-        <v>107</v>
+      <c r="A35" s="47" t="s">
+        <v>105</v>
       </c>
       <c r="B35" s="44">
         <v>0</v>
@@ -2760,7 +2780,7 @@
       <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="47" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="44">
@@ -2771,7 +2791,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="41">
         <v>1</v>
@@ -2781,7 +2801,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B38" s="41">
         <v>1</v>
@@ -2791,7 +2811,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" s="41">
         <v>1</v>
@@ -2865,7 +2885,7 @@
       <c r="A46" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="46">
+      <c r="B46" s="45">
         <f>B44/B45*100</f>
         <v>83.333333333333343</v>
       </c>
@@ -2876,11 +2896,11 @@
       <c r="A47" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
+      <c r="B47" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
@@ -3129,10 +3149,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3162,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -3153,10 +3173,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="57">
-        <v>0</v>
+        <v>133</v>
+      </c>
+      <c r="B2" s="49">
+        <v>1</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -3164,9 +3184,9 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="47">
+        <v>134</v>
+      </c>
+      <c r="B3" s="46">
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
@@ -3175,10 +3195,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="47">
-        <v>0</v>
+        <v>128</v>
+      </c>
+      <c r="B4" s="46">
+        <v>1</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -3186,10 +3206,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="47">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="B5" s="46">
+        <v>1</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -3197,10 +3217,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="47">
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="B6" s="46">
+        <v>1</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -3208,9 +3228,9 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="47">
+        <v>135</v>
+      </c>
+      <c r="B7" s="46">
         <v>1</v>
       </c>
       <c r="C7" s="19"/>
@@ -3219,9 +3239,9 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="47">
+        <v>136</v>
+      </c>
+      <c r="B8" s="46">
         <v>1</v>
       </c>
       <c r="C8" s="19"/>
@@ -3229,33 +3249,33 @@
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="47">
-        <v>0</v>
+      <c r="A9" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="46">
+        <v>1</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="47">
-        <v>0</v>
+      <c r="A10" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="46">
+        <v>1</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="47">
-        <v>0</v>
+      <c r="A11" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="46">
+        <v>1</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -3263,21 +3283,21 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="47">
-        <v>0</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B12" s="46">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="47">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="B13" s="46">
+        <v>1</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -3285,10 +3305,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="47">
-        <v>0</v>
+        <v>116</v>
+      </c>
+      <c r="B14" s="46">
+        <v>1</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -3296,32 +3316,32 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="47">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="B15" s="46">
+        <v>1</v>
       </c>
       <c r="D15" s="19"/>
-      <c r="E15" s="31"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="47">
-        <v>0</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="6"/>
+        <v>118</v>
+      </c>
+      <c r="B16" s="46">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="47">
-        <v>0</v>
+        <v>110</v>
+      </c>
+      <c r="B17" s="46">
+        <v>1</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
@@ -3329,10 +3349,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="47">
-        <v>0</v>
+        <v>111</v>
+      </c>
+      <c r="B18" s="46">
+        <v>1</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
@@ -3340,10 +3360,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="47">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="B19" s="46">
+        <v>1</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
@@ -3351,107 +3371,116 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="47">
+        <v>79</v>
+      </c>
+      <c r="B20" s="46">
         <v>0</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="D20" s="31"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="47">
+        <v>81</v>
+      </c>
+      <c r="B21" s="46">
         <v>0</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="47">
+        <v>82</v>
+      </c>
+      <c r="B22" s="46">
         <v>0</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="47">
-        <v>0</v>
+        <v>121</v>
+      </c>
+      <c r="B23" s="46">
+        <v>1</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="47">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="B24" s="46">
+        <v>1</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="47">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="B25" s="46">
+        <v>1</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="47">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="B26" s="46">
+        <v>1</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="47">
-        <v>0</v>
-      </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
+        <v>85</v>
+      </c>
+      <c r="B27" s="46">
+        <v>1</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="47">
-        <v>0</v>
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="46">
+        <v>1</v>
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="47">
-        <v>0</v>
-      </c>
+      <c r="B29" s="46">
+        <v>1</v>
+      </c>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="47">
+        <v>86</v>
+      </c>
+      <c r="B30" s="46">
         <v>0</v>
       </c>
     </row>
@@ -3459,145 +3488,143 @@
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="47">
-        <v>0</v>
+      <c r="B31" s="46">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" s="47">
+        <v>127</v>
+      </c>
+      <c r="B32" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="46">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="47">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="46">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="47">
+      <c r="C40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>129</v>
-      </c>
-      <c r="B36" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="13">
-        <f>SUM(B2:B43)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14" t="s">
+      <c r="B42" s="13">
+        <f>SUM(B2:B41)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="15">
-        <f>COUNT(B2:B43)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+      <c r="B43" s="15">
+        <f>COUNT(B2:B41)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="36">
-        <f>B44/B45*100</f>
-        <v>7.1428571428571423</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="B44" s="36">
+        <f>B42/B43*100</f>
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="37"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="37"/>
+      <c r="B45" s="37"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="37"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3658,14 +3685,6 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3697,7 +3716,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3707,7 +3726,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3717,7 +3736,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3727,7 +3746,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3737,7 +3756,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3747,7 +3766,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3767,7 +3786,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3906,7 +3925,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3917,7 +3936,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3928,7 +3947,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3950,7 +3969,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
updated task and bug metrics
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7470" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -20,17 +15,12 @@
     <sheet name="Iteration 5" sheetId="5" r:id="rId6"/>
     <sheet name="Iteration 6" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="162">
   <si>
     <t>Task</t>
   </si>
@@ -398,27 +388,6 @@
     <t>Smartphone overuse report JSON</t>
   </si>
   <si>
-    <t>Test smartphone overuse report</t>
-  </si>
-  <si>
-    <t>Debug smartphone overuse report</t>
-  </si>
-  <si>
-    <t>Slides for supervisor meeting</t>
-  </si>
-  <si>
-    <t>New testcases</t>
-  </si>
-  <si>
-    <t>Test all functions with new testcases</t>
-  </si>
-  <si>
-    <t>Debug based on nes test cases</t>
-  </si>
-  <si>
-    <t>Update Next iteration</t>
-  </si>
-  <si>
     <t>Match final submission with requirements</t>
   </si>
   <si>
@@ -547,13 +516,106 @@
   </si>
   <si>
     <t>Preparation of Material for supervisor Meeting</t>
+  </si>
+  <si>
+    <t>Building of additional Test Case for Top k</t>
+  </si>
+  <si>
+    <t>Debugging of Top-K report</t>
+  </si>
+  <si>
+    <t>Preparation of slides for Supervisor Meeting 3</t>
+  </si>
+  <si>
+    <t>Changes to Bootstrap (Location-Delete) (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Supervisor Meeting 3</t>
+  </si>
+  <si>
+    <t>Internal Meeting</t>
+  </si>
+  <si>
+    <t>Testing of Bootstrap - Delete Location Data (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>SOCIAL ACTIVENESS FUNCTION</t>
+  </si>
+  <si>
+    <t>Testing of Bootstrap additional Demographics (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Changes to Basic App Requirement (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Regressison Testing</t>
+  </si>
+  <si>
+    <t>Debugging of Basic App- Based on New test Cases (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Debugging of BootStrap Change in Demographics - Based on new Test Cases (Additional Change In Requirement)</t>
+  </si>
+  <si>
+    <t>Debugging of BootStrap Delete Location - Based on new Test Cases (Additional Change In Requirement)</t>
+  </si>
+  <si>
+    <t>Debugging of Social Activeness Report</t>
+  </si>
+  <si>
+    <t>Overall Integration before deployment</t>
+  </si>
+  <si>
+    <t>Testing of Bootstrap Basic App Function (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Testing of Social Activeness Function</t>
+  </si>
+  <si>
+    <t>Update Metric and Apply Mitigration</t>
+  </si>
+  <si>
+    <t>Revise Diagrams</t>
+  </si>
+  <si>
+    <t>Code Sharing</t>
+  </si>
+  <si>
+    <t>PM Handover (Knowledge transfer on schedule, metrics, admin etc)</t>
+  </si>
+  <si>
+    <t>Update next iteration schedule</t>
+  </si>
+  <si>
+    <t>User Acceptance Test</t>
+  </si>
+  <si>
+    <t>Testing of Top k report</t>
+  </si>
+  <si>
+    <t>Building New Test Cases for Bootstrap change of demographic field (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Building Test Cases for Social Activeness Function</t>
+  </si>
+  <si>
+    <t>Building of new Test Cases for Basic Add based on (Additional Change in Rerquiremenr</t>
+  </si>
+  <si>
+    <t>Changes to Bootstrap - Additional Demographics (CCA) (Additional Change in Requirement)</t>
+  </si>
+  <si>
+    <t>Debugging of Heatmap</t>
+  </si>
+  <si>
+    <t>Debugging of Overuse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +652,43 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1013,10 +1112,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1142,18 +1242,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1414,7 +1522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1428,12 +1536,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="98.140625" customWidth="1"/>
+    <col min="2" max="2" width="98.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="24" thickTop="1" thickBot="1">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -1441,7 +1549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="22.5" customHeight="1">
       <c r="A2" s="52" t="s">
         <v>16</v>
       </c>
@@ -1449,13 +1557,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.649999999999999" customHeight="1" thickBot="1">
       <c r="A3" s="53"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="14.15" customHeight="1">
       <c r="A4" s="52" t="s">
         <v>17</v>
       </c>
@@ -1463,19 +1571,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" customHeight="1">
       <c r="A5" s="54"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.15" customHeight="1" thickBot="1">
       <c r="A6" s="53"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" s="52" t="s">
         <v>18</v>
       </c>
@@ -1483,19 +1591,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="22.5" customHeight="1">
       <c r="A8" s="54"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="53"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="24" customHeight="1">
       <c r="A10" s="52" t="s">
         <v>20</v>
       </c>
@@ -1503,19 +1611,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="54"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1">
       <c r="A12" s="53"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="28" customHeight="1">
       <c r="A13" s="52" t="s">
         <v>22</v>
       </c>
@@ -1523,13 +1631,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1">
       <c r="A14" s="55"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
@@ -1550,18 +1658,18 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="94.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="67.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="94.26953125" customWidth="1"/>
+    <col min="6" max="6" width="32.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1680,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1584,7 +1692,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1596,7 +1704,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1608,7 +1716,7 @@
       <c r="E4" s="31"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1620,7 +1728,7 @@
       <c r="E5" s="32"/>
       <c r="F5" s="30"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1740,7 @@
       <c r="E6" s="32"/>
       <c r="F6" s="30"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1644,7 +1752,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="30"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1656,7 +1764,7 @@
       <c r="E8" s="32"/>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1668,7 +1776,7 @@
       <c r="E9" s="32"/>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1681,7 +1789,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="30"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1694,7 +1802,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -1707,19 +1815,19 @@
       <c r="E12" s="33"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="14.5" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="3"/>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>
@@ -1727,7 +1835,7 @@
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="3"/>
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
@@ -1735,7 +1843,7 @@
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="3"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -1743,7 +1851,7 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15">
       <c r="A17" s="3"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -1751,7 +1859,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="3"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1759,7 +1867,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="30"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -1767,7 +1875,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="19"/>
@@ -1775,332 +1883,332 @@
       <c r="E20" s="19"/>
       <c r="F20" s="30"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="3"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="3"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="3"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="3"/>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="3"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="3"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="3"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="3"/>
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="3"/>
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="3"/>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="3"/>
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="3"/>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="3"/>
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="3"/>
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="3"/>
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="3"/>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="3"/>
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="3"/>
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="3"/>
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="3"/>
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="3"/>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="3"/>
       <c r="B64" s="6"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="3"/>
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="3"/>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="3"/>
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="3"/>
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="3"/>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="3"/>
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="3"/>
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="3"/>
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="3"/>
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="3"/>
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="3"/>
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="3"/>
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" s="3"/>
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" s="3"/>
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="3"/>
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" s="3"/>
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="3"/>
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="3"/>
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="3"/>
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="3"/>
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="3"/>
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="3"/>
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="3"/>
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="3"/>
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" s="3"/>
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="3"/>
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="3"/>
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" s="3"/>
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" s="3"/>
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="3"/>
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="3"/>
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="3"/>
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="3"/>
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="3"/>
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" ht="15" thickBot="1">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="B101" s="6"/>
     </row>
   </sheetData>
@@ -2120,13 +2228,13 @@
       <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2136,7 +2244,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -2148,7 +2256,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -2160,7 +2268,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2172,7 +2280,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -2184,7 +2292,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2196,7 +2304,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -2206,7 +2314,7 @@
       <c r="C7" s="19"/>
       <c r="D7" s="31"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2216,7 +2324,7 @@
       <c r="C8" s="19"/>
       <c r="D8" s="31"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2226,7 +2334,7 @@
       <c r="C9" s="19"/>
       <c r="D9" s="31"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2344,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -2246,7 +2354,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2256,7 +2364,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -2266,7 +2374,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -2276,7 +2384,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2286,7 +2394,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -2296,7 +2404,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -2306,7 +2414,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -2316,7 +2424,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2434,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>11</v>
       </c>
@@ -2337,7 +2445,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
@@ -2348,7 +2456,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="17" t="s">
         <v>13</v>
       </c>
@@ -2359,23 +2467,23 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="3"/>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="3"/>
       <c r="B25" s="56"/>
       <c r="C25" s="56"/>
@@ -2393,16 +2501,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A36"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2520,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -2425,7 +2533,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -2438,7 +2546,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
@@ -2451,7 +2559,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
@@ -2464,7 +2572,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="39" t="s">
         <v>43</v>
       </c>
@@ -2477,7 +2585,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -2490,7 +2598,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -2503,7 +2611,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
@@ -2516,7 +2624,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -2529,7 +2637,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -2539,7 +2647,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2549,7 +2657,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15">
       <c r="A13" s="3" t="s">
         <v>54</v>
       </c>
@@ -2559,7 +2667,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -2569,7 +2677,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -2579,7 +2687,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -2589,7 +2697,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2599,7 +2707,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2609,7 +2717,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="39" t="s">
         <v>62</v>
       </c>
@@ -2619,7 +2727,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="39" t="s">
         <v>61</v>
       </c>
@@ -2629,7 +2737,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="39" t="s">
         <v>63</v>
       </c>
@@ -2639,7 +2747,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="47" t="s">
         <v>73</v>
       </c>
@@ -2649,9 +2757,9 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="47" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B23" s="4">
         <v>0</v>
@@ -2659,7 +2767,7 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="39" t="s">
         <v>64</v>
       </c>
@@ -2669,7 +2777,7 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="39" t="s">
         <v>65</v>
       </c>
@@ -2679,7 +2787,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="39" t="s">
         <v>67</v>
       </c>
@@ -2689,7 +2797,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="39" t="s">
         <v>68</v>
       </c>
@@ -2699,7 +2807,7 @@
       <c r="C27" s="19"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="39" t="s">
         <v>66</v>
       </c>
@@ -2709,7 +2817,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="47" t="s">
         <v>69</v>
       </c>
@@ -2719,7 +2827,7 @@
       <c r="C29" s="19"/>
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" s="47" t="s">
         <v>71</v>
       </c>
@@ -2729,7 +2837,7 @@
       <c r="C30" s="19"/>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" s="47" t="s">
         <v>72</v>
       </c>
@@ -2739,7 +2847,7 @@
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="39" t="s">
         <v>46</v>
       </c>
@@ -2749,9 +2857,9 @@
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="39" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B33" s="44">
         <v>1</v>
@@ -2759,7 +2867,7 @@
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="39" t="s">
         <v>75</v>
       </c>
@@ -2769,9 +2877,9 @@
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="47" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B35" s="44">
         <v>0</v>
@@ -2779,7 +2887,7 @@
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="47" t="s">
         <v>70</v>
       </c>
@@ -2789,7 +2897,7 @@
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="39" t="s">
         <v>84</v>
       </c>
@@ -2799,9 +2907,9 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="39" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B38" s="41">
         <v>1</v>
@@ -2809,9 +2917,9 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="39" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B39" s="41">
         <v>1</v>
@@ -2819,7 +2927,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="39" t="s">
         <v>76</v>
       </c>
@@ -2829,7 +2937,7 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="39" t="s">
         <v>74</v>
       </c>
@@ -2839,7 +2947,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="39" t="s">
         <v>9</v>
       </c>
@@ -2849,7 +2957,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" thickBot="1">
       <c r="A43" s="39" t="s">
         <v>77</v>
       </c>
@@ -2859,7 +2967,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
@@ -2870,7 +2978,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15.5" thickTop="1" thickBot="1">
       <c r="A45" s="14" t="s">
         <v>12</v>
       </c>
@@ -2881,7 +2989,7 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.5" thickTop="1" thickBot="1">
       <c r="A46" s="43" t="s">
         <v>13</v>
       </c>
@@ -2892,251 +3000,251 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="87.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="88" customHeight="1" thickTop="1" thickBot="1">
       <c r="A47" s="42" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="57" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C47" s="58"/>
       <c r="D47" s="58"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" thickTop="1">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1">
       <c r="A89" s="6"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" s="6"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1">
       <c r="A91" s="6"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1">
       <c r="A92" s="6"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1">
       <c r="A93" s="6"/>
     </row>
   </sheetData>
@@ -3151,17 +3259,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="79.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="79.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3171,9 +3279,9 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B2" s="49">
         <v>1</v>
@@ -3182,9 +3290,9 @@
       <c r="D2" s="19"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B3" s="46">
         <v>1</v>
@@ -3193,9 +3301,9 @@
       <c r="D3" s="19"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B4" s="46">
         <v>1</v>
@@ -3204,9 +3312,9 @@
       <c r="D4" s="19"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B5" s="46">
         <v>1</v>
@@ -3215,9 +3323,9 @@
       <c r="D5" s="19"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B6" s="46">
         <v>1</v>
@@ -3226,9 +3334,9 @@
       <c r="D6" s="19"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B7" s="46">
         <v>1</v>
@@ -3237,9 +3345,9 @@
       <c r="D7" s="19"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B8" s="46">
         <v>1</v>
@@ -3248,9 +3356,9 @@
       <c r="D8" s="19"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="30" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B9" s="46">
         <v>1</v>
@@ -3259,9 +3367,9 @@
       <c r="D9" s="19"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="50" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B10" s="46">
         <v>1</v>
@@ -3270,9 +3378,9 @@
       <c r="D10" s="19"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="51" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B11" s="46">
         <v>1</v>
@@ -3281,9 +3389,9 @@
       <c r="D11" s="19"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B12" s="46">
         <v>1</v>
@@ -3292,9 +3400,9 @@
       <c r="D12" s="19"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B13" s="46">
         <v>1</v>
@@ -3303,9 +3411,9 @@
       <c r="E13" s="19"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B14" s="46">
         <v>1</v>
@@ -3314,9 +3422,9 @@
       <c r="E14" s="19"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B15" s="46">
         <v>1</v>
@@ -3325,9 +3433,9 @@
       <c r="E15" s="19"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B16" s="46">
         <v>1</v>
@@ -3336,9 +3444,9 @@
       <c r="E16" s="31"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B17" s="46">
         <v>1</v>
@@ -3347,9 +3455,9 @@
       <c r="D17" s="31"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B18" s="46">
         <v>1</v>
@@ -3358,7 +3466,7 @@
       <c r="D18" s="31"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -3369,7 +3477,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -3377,12 +3485,12 @@
         <v>0</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -3390,11 +3498,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -3402,13 +3510,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B23" s="46">
         <v>1</v>
@@ -3416,9 +3524,9 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B24" s="46">
         <v>1</v>
@@ -3426,9 +3534,9 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B25" s="46">
         <v>1</v>
@@ -3436,7 +3544,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3446,7 +3554,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -3456,7 +3564,7 @@
       <c r="C27" s="19"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -3466,7 +3574,7 @@
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15">
       <c r="A29" s="39" t="s">
         <v>88</v>
       </c>
@@ -3476,7 +3584,7 @@
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15">
       <c r="A30" s="6" t="s">
         <v>86</v>
       </c>
@@ -3484,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15">
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
@@ -3492,15 +3600,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15">
       <c r="A32" s="30" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B32" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -3508,77 +3616,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B37" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>119</v>
-      </c>
       <c r="B38" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B39" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B40" s="46">
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
       <c r="A42" s="10" t="s">
         <v>11</v>
       </c>
@@ -3587,7 +3695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15" thickBot="1">
       <c r="A43" s="14" t="s">
         <v>12</v>
       </c>
@@ -3596,7 +3704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.5" thickTop="1" thickBot="1">
       <c r="A44" s="17" t="s">
         <v>13</v>
       </c>
@@ -3605,85 +3713,85 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="37"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="37"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="6"/>
     </row>
   </sheetData>
@@ -3694,19 +3802,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="81.85546875" customWidth="1"/>
+    <col min="1" max="1" width="123" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3714,49 +3822,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+    <row r="2" spans="1:5" ht="15.5">
+      <c r="A2" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="59">
+        <v>1</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0</v>
+    <row r="3" spans="1:5" ht="15.5">
+      <c r="A3" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="66">
+        <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="4">
+    <row r="4" spans="1:5" ht="15.5">
+      <c r="A4" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="66">
         <v>0</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
+    <row r="5" spans="1:5" ht="15.5">
+      <c r="A5" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="66">
+        <v>1</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
+    <row r="6" spans="1:5" ht="15.5">
+      <c r="A6" s="62" t="s">
+        <v>134</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3764,9 +3872,9 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>94</v>
+    <row r="7" spans="1:5" ht="15.5">
+      <c r="A7" s="62" t="s">
+        <v>135</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3774,9 +3882,9 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
+    <row r="8" spans="1:5" ht="15.5">
+      <c r="A8" s="61" t="s">
+        <v>156</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -3784,9 +3892,9 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>95</v>
+    <row r="9" spans="1:5" ht="15.5">
+      <c r="A9" s="61" t="s">
+        <v>157</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -3794,104 +3902,248 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+    <row r="10" spans="1:5" ht="15.5">
+      <c r="A10" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+    <row r="11" spans="1:5" ht="15.5">
+      <c r="A11" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.5">
+      <c r="A12" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="16" thickBot="1">
+      <c r="A13" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.5">
+      <c r="A14" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.5">
+      <c r="A15" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.5">
+      <c r="A16" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5">
+      <c r="A17" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.5">
+      <c r="A18" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5">
+      <c r="A19" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5">
+      <c r="A20" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickBot="1">
+      <c r="A21" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5">
+      <c r="A22" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5">
+      <c r="A23" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5">
+      <c r="A24" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5">
+      <c r="A25" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5">
+      <c r="A26" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5">
+      <c r="A27" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5">
+      <c r="A28" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5">
+      <c r="A29" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16.5">
+      <c r="A30" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5">
+      <c r="A31" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16.5">
+      <c r="A32" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5">
+      <c r="A33" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5">
+      <c r="A34" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1">
+      <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="13">
-        <f>SUM(B2:B25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="B35" s="13">
+        <f>SUM(B2:B34)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A36" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="15">
-        <f>COUNT(B2:B25)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="B36" s="15">
+        <f>COUNT(B2:B34)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="36">
-        <f>B26/B27*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="B37" s="36">
+        <f>B35/B36*100</f>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15">
+      <c r="A38" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="37"/>
+      <c r="B38" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3902,17 +4154,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="76.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="76.26953125" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3923,9 +4175,9 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3934,9 +4186,9 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3945,9 +4197,9 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3956,7 +4208,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -3967,9 +4219,9 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -3978,95 +4230,95 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -4075,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="14" t="s">
         <v>12</v>
       </c>
@@ -4084,7 +4336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A28" s="17" t="s">
         <v>13</v>
       </c>
@@ -4093,18 +4345,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="37"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>

</xml_diff>

<commit_message>
updated bugs and task metrics for iteration 5
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7470" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7470" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -1221,6 +1221,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1242,16 +1252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1522,7 +1522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1550,7 +1550,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="22.5" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="60" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1558,13 +1558,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.649999999999999" customHeight="1" thickBot="1">
-      <c r="A3" s="53"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.15" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="60" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -1572,19 +1572,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1">
-      <c r="A5" s="54"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.15" customHeight="1" thickBot="1">
-      <c r="A6" s="53"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="60" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1592,19 +1592,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" customHeight="1">
-      <c r="A8" s="54"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1">
-      <c r="A9" s="53"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" customHeight="1">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="60" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1612,19 +1612,19 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="54"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1">
-      <c r="A12" s="53"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28" customHeight="1">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="60" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -1632,12 +1632,12 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1">
-      <c r="A14" s="55"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickTop="1"/>
+    <row r="15" spans="1:2" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
@@ -1669,7 +1669,7 @@
     <col min="7" max="7" width="7.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="E4" s="31"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="E5" s="32"/>
       <c r="F5" s="30"/>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="E6" s="32"/>
       <c r="F6" s="30"/>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="30"/>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="E8" s="32"/>
       <c r="F8" s="30"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+    <row r="9" spans="1:6" ht="15" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="E9" s="32"/>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
+    <row r="10" spans="1:6" ht="15.5" thickTop="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="30"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+    <row r="11" spans="1:6" ht="15" thickBot="1">
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
+    <row r="12" spans="1:6" ht="15.5" thickTop="1" thickBot="1">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -1819,31 +1819,31 @@
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6">
       <c r="A16" s="3"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -1851,7 +1851,7 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6">
       <c r="A17" s="3"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -1859,7 +1859,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="30"/>
     </row>
-    <row r="18" spans="1:6" ht="15">
+    <row r="18" spans="1:6">
       <c r="A18" s="3"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1867,7 +1867,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="30"/>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6">
       <c r="A19" s="3"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -1875,7 +1875,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="30"/>
     </row>
-    <row r="20" spans="1:6" ht="15">
+    <row r="20" spans="1:6">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="19"/>
@@ -1883,33 +1883,33 @@
       <c r="E20" s="19"/>
       <c r="F20" s="30"/>
     </row>
-    <row r="21" spans="1:6" ht="15">
+    <row r="21" spans="1:6">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:6" ht="15">
+    <row r="22" spans="1:6">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:6" ht="15">
+    <row r="23" spans="1:6">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="15">
+    <row r="24" spans="1:6">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="15">
+    <row r="25" spans="1:6">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15">
+    <row r="26" spans="1:6">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
     </row>
@@ -2234,7 +2234,7 @@
     <col min="2" max="2" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -2256,7 +2256,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2280,7 +2280,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -2304,7 +2304,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="C7" s="19"/>
       <c r="D7" s="31"/>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="C8" s="19"/>
       <c r="D8" s="31"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="C9" s="19"/>
       <c r="D9" s="31"/>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="C10" s="19"/>
       <c r="D10" s="31"/>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -2384,7 +2384,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -2394,7 +2394,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -2404,7 +2404,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+    <row r="19" spans="1:4" ht="15" thickBot="1">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+    <row r="20" spans="1:4" ht="15.5" thickTop="1" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>11</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+    <row r="21" spans="1:4" ht="15" thickBot="1">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
@@ -2456,7 +2456,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+    <row r="22" spans="1:4" ht="15.5" thickTop="1" thickBot="1">
       <c r="A22" s="17" t="s">
         <v>13</v>
       </c>
@@ -2471,23 +2471,23 @@
       <c r="A23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2510,7 +2510,7 @@
     <col min="1" max="1" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -2546,7 +2546,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7">
       <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
@@ -2559,7 +2559,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7">
       <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
@@ -2572,7 +2572,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7">
       <c r="A6" s="39" t="s">
         <v>43</v>
       </c>
@@ -2585,7 +2585,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="15">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -2637,7 +2637,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="C11" s="19"/>
       <c r="D11" s="31"/>
     </row>
-    <row r="12" spans="1:7" ht="15">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="C12" s="19"/>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:7" ht="15">
+    <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>54</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="31"/>
     </row>
-    <row r="14" spans="1:7" ht="15">
+    <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="31"/>
     </row>
-    <row r="15" spans="1:7" ht="15">
+    <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="C15" s="19"/>
       <c r="D15" s="31"/>
     </row>
-    <row r="16" spans="1:7" ht="15">
+    <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="31"/>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2717,7 +2717,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4">
       <c r="A19" s="39" t="s">
         <v>62</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4">
       <c r="A20" s="39" t="s">
         <v>61</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4">
       <c r="A21" s="39" t="s">
         <v>63</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4">
       <c r="A22" s="47" t="s">
         <v>73</v>
       </c>
@@ -2757,7 +2757,7 @@
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4">
       <c r="A23" s="47" t="s">
         <v>97</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4">
       <c r="A24" s="39" t="s">
         <v>64</v>
       </c>
@@ -2777,7 +2777,7 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4">
       <c r="A25" s="39" t="s">
         <v>65</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4">
       <c r="A26" s="39" t="s">
         <v>67</v>
       </c>
@@ -2797,7 +2797,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4">
       <c r="A27" s="39" t="s">
         <v>68</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="C27" s="19"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4">
       <c r="A28" s="39" t="s">
         <v>66</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="C28" s="19"/>
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4">
       <c r="A29" s="47" t="s">
         <v>69</v>
       </c>
@@ -2827,7 +2827,7 @@
       <c r="C29" s="19"/>
       <c r="D29" s="31"/>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4">
       <c r="A30" s="47" t="s">
         <v>71</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="C30" s="19"/>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4">
       <c r="A31" s="47" t="s">
         <v>72</v>
       </c>
@@ -3004,11 +3004,11 @@
       <c r="A47" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
     </row>
     <row r="48" spans="1:4" ht="15" thickTop="1">
       <c r="A48" s="6"/>
@@ -3269,7 +3269,7 @@
     <col min="9" max="9" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3279,7 +3279,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="D2" s="19"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c r="D3" s="19"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>122</v>
       </c>
@@ -3323,7 +3323,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>123</v>
       </c>
@@ -3334,7 +3334,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>128</v>
       </c>
@@ -3345,7 +3345,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>129</v>
       </c>
@@ -3356,7 +3356,7 @@
       <c r="D8" s="19"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="30" t="s">
         <v>130</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6">
       <c r="A10" s="50" t="s">
         <v>117</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6">
       <c r="A11" s="51" t="s">
         <v>101</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="D12" s="19"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>109</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -3433,7 +3433,7 @@
       <c r="E15" s="19"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -3444,7 +3444,7 @@
       <c r="E16" s="31"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -3455,7 +3455,7 @@
       <c r="D17" s="31"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -3466,7 +3466,7 @@
       <c r="D18" s="31"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -3477,7 +3477,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -3490,7 +3490,7 @@
       <c r="D20" s="31"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="C23" s="19"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>115</v>
       </c>
@@ -3534,7 +3534,7 @@
       <c r="C24" s="19"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -3544,7 +3544,7 @@
       <c r="C25" s="19"/>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3554,7 +3554,7 @@
       <c r="C26" s="19"/>
       <c r="D26" s="31"/>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="C27" s="19"/>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:5" ht="15">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5">
       <c r="A29" s="39" t="s">
         <v>88</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
     </row>
-    <row r="30" spans="1:5" ht="15">
+    <row r="30" spans="1:5">
       <c r="A30" s="6" t="s">
         <v>86</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5">
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5">
       <c r="A32" s="30" t="s">
         <v>120</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -3804,8 +3804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3823,257 +3823,257 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="52">
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="15.5">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="66">
+      <c r="B3" s="59">
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="15.5">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="66">
-        <v>0</v>
+      <c r="B4" s="59">
+        <v>1</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="15.5">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="66">
+      <c r="B5" s="59">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="15.5">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="55" t="s">
         <v>134</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.5">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="55" t="s">
         <v>135</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="15.5">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="54" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15.5">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="54" t="s">
         <v>157</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15.5">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="54" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="15.5">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="54" t="s">
         <v>159</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="15.5">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="54" t="s">
         <v>160</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="54" t="s">
         <v>161</v>
       </c>
       <c r="B13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="15.5">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="55" t="s">
         <v>136</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" ht="15.5">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="57" t="s">
         <v>137</v>
       </c>
       <c r="B15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.5">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="56" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.5">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="57" t="s">
         <v>139</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="55" t="s">
         <v>140</v>
       </c>
       <c r="B18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="58" t="s">
         <v>141</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="58" t="s">
         <v>142</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17" thickBot="1">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="58" t="s">
         <v>143</v>
       </c>
       <c r="B21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="58" t="s">
         <v>144</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="58" t="s">
         <v>145</v>
       </c>
       <c r="B23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="58" t="s">
         <v>95</v>
       </c>
       <c r="B24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16.5">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="58" t="s">
         <v>146</v>
       </c>
       <c r="B25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="58" t="s">
         <v>147</v>
       </c>
       <c r="B26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16.5">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="58" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16.5">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="58" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16.5">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="58" t="s">
         <v>150</v>
       </c>
       <c r="B29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16.5">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="58" t="s">
         <v>151</v>
       </c>
       <c r="B30" s="4">
@@ -4081,7 +4081,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="16.5">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="58" t="s">
         <v>136</v>
       </c>
       <c r="B31" s="4">
@@ -4089,7 +4089,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="58" t="s">
         <v>152</v>
       </c>
       <c r="B32" s="4">
@@ -4097,7 +4097,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="58" t="s">
         <v>153</v>
       </c>
       <c r="B33" s="4">
@@ -4105,7 +4105,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="58" t="s">
         <v>154</v>
       </c>
       <c r="B34" s="4">
@@ -4118,10 +4118,10 @@
       </c>
       <c r="B35" s="13">
         <f>SUM(B2:B34)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1">
       <c r="A36" s="14" t="s">
         <v>12</v>
       </c>
@@ -4130,16 +4130,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+    <row r="37" spans="1:2" ht="15.5" thickTop="1" thickBot="1">
       <c r="A37" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="36">
         <f>B35/B36*100</f>
-        <v>9.0909090909090917</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15">
+        <v>115.15151515151516</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="8" t="s">
         <v>2</v>
       </c>
@@ -4154,7 +4154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -4164,7 +4164,7 @@
     <col min="2" max="2" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4175,7 +4175,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>90</v>
       </c>
@@ -4197,7 +4197,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>91</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -4219,7 +4219,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>92</v>
       </c>
@@ -4230,95 +4230,95 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="15">
+    <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="15">
+    <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+    <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="26" spans="1:3" ht="15.5" thickTop="1" thickBot="1">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+    <row r="27" spans="1:3" ht="15" thickBot="1">
       <c r="A27" s="14" t="s">
         <v>12</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="28" spans="1:3" ht="15.5" thickTop="1" thickBot="1">
       <c r="A28" s="17" t="s">
         <v>13</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Task Metrics revised for the day
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15460" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -1641,7 +1641,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4304,7 +4304,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4394,7 +4394,9 @@
       <c r="A8" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -4403,7 +4405,9 @@
       <c r="A9" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4412,7 +4416,9 @@
       <c r="A10" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -4421,61 +4427,81 @@
       <c r="A11" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
@@ -4585,7 +4611,7 @@
       </c>
       <c r="B38" s="13">
         <f>SUM(B2:B37)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1">
@@ -4594,7 +4620,7 @@
       </c>
       <c r="B39" s="15">
         <f>COUNT(B2:B37)</f>
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" thickTop="1" thickBot="1">
@@ -4603,7 +4629,7 @@
       </c>
       <c r="B40" s="36">
         <f>B38/B39*100</f>
-        <v>83.333333333333343</v>
+        <v>63.157894736842103</v>
       </c>
     </row>
     <row r="41" spans="1:3">

</xml_diff>

<commit_message>
Final task metric update
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="193">
   <si>
     <t>Task</t>
   </si>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>Final Submission</t>
+  </si>
+  <si>
+    <t>Celebration</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1234,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1366,6 +1369,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1641,7 +1647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4303,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4329,7 +4335,7 @@
         <v>158</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -4395,7 +4401,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -4428,7 +4434,7 @@
         <v>167</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4436,7 +4442,7 @@
         <v>168</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4476,7 +4482,7 @@
         <v>173</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4484,7 +4490,7 @@
         <v>174</v>
       </c>
       <c r="B18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4500,110 +4506,144 @@
         <v>176</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1">
       <c r="A38" s="10" t="s">
@@ -4611,7 +4651,7 @@
       </c>
       <c r="B38" s="13">
         <f>SUM(B2:B37)</f>
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1">
@@ -4620,7 +4660,7 @@
       </c>
       <c r="B39" s="15">
         <f>COUNT(B2:B37)</f>
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" thickTop="1" thickBot="1">
@@ -4629,7 +4669,7 @@
       </c>
       <c r="B40" s="36">
         <f>B38/B39*100</f>
-        <v>63.157894736842103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -4639,7 +4679,9 @@
       <c r="B41" s="37"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="67" t="s">
+        <v>192</v>
+      </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>

</xml_diff>

<commit_message>
Updated task metric for consistency with plug
</commit_message>
<xml_diff>
--- a/metrics/Task Metrics with Mitigation Plan.xlsx
+++ b/metrics/Task Metrics with Mitigation Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Mitigation Metrics" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="197">
   <si>
     <t>Task</t>
   </si>
@@ -707,6 +707,18 @@
   </si>
   <si>
     <t>Celebration</t>
+  </si>
+  <si>
+    <t>Supervisor meeting</t>
+  </si>
+  <si>
+    <t>Internal meeting 1</t>
+  </si>
+  <si>
+    <t>Internal meeting</t>
+  </si>
+  <si>
+    <t>Internal meeting w/ PM Handover</t>
   </si>
 </sst>
 </file>
@@ -752,13 +764,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -783,12 +788,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -804,8 +803,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -839,12 +849,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,15 +1230,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1330,7 +1346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1339,16 +1354,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1370,15 +1385,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1647,7 +1674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1675,7 +1702,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="22.5" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1683,13 +1710,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -1697,19 +1724,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1">
-      <c r="A5" s="62"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A6" s="61"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1717,19 +1744,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" customHeight="1">
-      <c r="A8" s="62"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="22" customHeight="1" thickBot="1">
-      <c r="A9" s="61"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="27" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" customHeight="1">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1737,19 +1764,19 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="62"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="22" customHeight="1" thickBot="1">
-      <c r="A12" s="61"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28" customHeight="1">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="57" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="22" t="s">
@@ -1757,7 +1784,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.5" customHeight="1" thickBot="1">
-      <c r="A14" s="63"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
@@ -1785,7 +1812,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1949,27 +1976,27 @@
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="32"/>
       <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="32"/>
       <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
       <c r="E15" s="32"/>
       <c r="F15" s="30"/>
     </row>
@@ -2357,10 +2384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2551,7 +2578,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -2559,76 +2586,97 @@
       <c r="C18" s="19"/>
       <c r="D18" s="31"/>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="31"/>
     </row>
-    <row r="20" spans="1:4" ht="16" thickTop="1" thickBot="1">
-      <c r="A20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="13">
-        <f>SUM(B2:B19)</f>
-        <v>13</v>
+    <row r="20" spans="1:4">
+      <c r="A20" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
-      <c r="A21" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="15">
-        <f>COUNT(B2:B19)</f>
-        <v>18</v>
+    <row r="21" spans="1:4">
+      <c r="A21" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="31"/>
     </row>
-    <row r="22" spans="1:4" ht="16" thickTop="1" thickBot="1">
-      <c r="A22" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="36">
-        <f>B20/B21*100</f>
-        <v>72.222222222222214</v>
+    <row r="22" spans="1:4" ht="15" thickBot="1">
+      <c r="A22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="13">
+        <f>SUM(B2:B21)</f>
+        <v>15</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:4" ht="15" thickBot="1">
+      <c r="A23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="15">
+        <f>COUNT(B2:B21)</f>
+        <v>20</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="31"/>
+    </row>
+    <row r="24" spans="1:4" ht="16" thickTop="1" thickBot="1">
+      <c r="A24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="36">
+        <f>B22/B23*100</f>
+        <v>75</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="31"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B25" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B23:D25"/>
+    <mergeCell ref="B25:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2639,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2888,7 +2936,7 @@
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="39" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="4">
@@ -2898,7 +2946,7 @@
       <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="39" t="s">
         <v>93</v>
       </c>
       <c r="B23" s="4">
@@ -2958,7 +3006,7 @@
       <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="39" t="s">
         <v>69</v>
       </c>
       <c r="B29" s="41">
@@ -2968,7 +3016,7 @@
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="39" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="41">
@@ -2978,7 +3026,7 @@
       <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="39" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="44">
@@ -3018,7 +3066,7 @@
       <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="39" t="s">
         <v>94</v>
       </c>
       <c r="B35" s="44">
@@ -3028,7 +3076,7 @@
       <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="39" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="44">
@@ -3097,9 +3145,9 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1">
+    <row r="43" spans="1:4">
       <c r="A43" s="39" t="s">
-        <v>77</v>
+        <v>195</v>
       </c>
       <c r="B43" s="41">
         <v>1</v>
@@ -3108,55 +3156,59 @@
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" ht="15" thickBot="1">
-      <c r="A44" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="15">
-        <f>SUM(B2:B43)</f>
-        <v>35</v>
+      <c r="A44" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="41">
+        <v>1</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="16" thickTop="1" thickBot="1">
-      <c r="A45" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="16">
-        <f>COUNT(B2:B43)</f>
-        <v>42</v>
+    <row r="45" spans="1:4" ht="15" thickBot="1">
+      <c r="A45" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="15">
+        <f>SUM(B2:B44)</f>
+        <v>36</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4" ht="16" thickTop="1" thickBot="1">
-      <c r="A46" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="45">
-        <f>B44/B45*100</f>
-        <v>83.333333333333343</v>
+      <c r="A46" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="16">
+        <f>COUNT(B2:B44)</f>
+        <v>43</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="88" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="42" t="s">
+    <row r="47" spans="1:4" ht="16" thickTop="1" thickBot="1">
+      <c r="A47" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="45">
+        <f>B45/B46*100</f>
+        <v>83.720930232558146</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" ht="88" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A48" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="65" t="s">
+      <c r="B48" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickTop="1">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickTop="1">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -3348,48 +3400,54 @@
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:4">
       <c r="A81" s="6"/>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:4">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:4">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:4">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:4">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:4">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:4">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:4">
       <c r="A89" s="6"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:4">
       <c r="A90" s="6"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:4">
       <c r="A91" s="6"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:4">
       <c r="A92" s="6"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:4">
       <c r="A93" s="6"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3404,7 +3462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -3415,7 +3473,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -3428,7 +3486,7 @@
       <c r="A2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="48">
         <v>1</v>
       </c>
       <c r="C2" s="19"/>
@@ -3513,7 +3571,7 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="49" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="46">
@@ -3524,7 +3582,7 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="46">
@@ -3954,8 +4012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3973,47 +4031,47 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="65">
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="66">
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="66">
         <v>1</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="66">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="52" t="s">
         <v>130</v>
       </c>
       <c r="B6" s="4">
@@ -4023,7 +4081,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="52" t="s">
         <v>131</v>
       </c>
       <c r="B7" s="4">
@@ -4033,7 +4091,7 @@
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="51" t="s">
         <v>152</v>
       </c>
       <c r="B8" s="4">
@@ -4043,7 +4101,7 @@
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="51" t="s">
         <v>153</v>
       </c>
       <c r="B9" s="4">
@@ -4053,7 +4111,7 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="51" t="s">
         <v>154</v>
       </c>
       <c r="B10" s="4">
@@ -4063,7 +4121,7 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="51" t="s">
         <v>155</v>
       </c>
       <c r="B11" s="4">
@@ -4073,7 +4131,7 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="51" t="s">
         <v>156</v>
       </c>
       <c r="B12" s="4">
@@ -4082,8 +4140,8 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1">
-      <c r="A13" s="54" t="s">
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="51" t="s">
         <v>157</v>
       </c>
       <c r="B13" s="4">
@@ -4093,17 +4151,17 @@
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="54" t="s">
         <v>133</v>
       </c>
       <c r="B15" s="4">
@@ -4111,7 +4169,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="53" t="s">
         <v>134</v>
       </c>
       <c r="B16" s="4">
@@ -4119,7 +4177,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="54" t="s">
         <v>135</v>
       </c>
       <c r="B17" s="4">
@@ -4127,7 +4185,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="52" t="s">
         <v>136</v>
       </c>
       <c r="B18" s="4">
@@ -4135,7 +4193,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="16">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="55" t="s">
         <v>137</v>
       </c>
       <c r="B19" s="4">
@@ -4143,15 +4201,15 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="16">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="55" t="s">
         <v>138</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" thickBot="1">
-      <c r="A21" s="58" t="s">
+    <row r="21" spans="1:2" ht="16">
+      <c r="A21" s="55" t="s">
         <v>139</v>
       </c>
       <c r="B21" s="4">
@@ -4159,15 +4217,15 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="16">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="55" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="55" t="s">
         <v>141</v>
       </c>
       <c r="B23" s="4">
@@ -4175,7 +4233,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="16">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="55" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="4">
@@ -4183,7 +4241,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="16">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="55" t="s">
         <v>142</v>
       </c>
       <c r="B25" s="4">
@@ -4191,7 +4249,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="16">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="55" t="s">
         <v>143</v>
       </c>
       <c r="B26" s="4">
@@ -4199,7 +4257,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="55" t="s">
         <v>144</v>
       </c>
       <c r="B27" s="4">
@@ -4207,7 +4265,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="16">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="55" t="s">
         <v>145</v>
       </c>
       <c r="B28" s="4">
@@ -4215,7 +4273,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="16">
-      <c r="A29" s="58" t="s">
+      <c r="A29" s="55" t="s">
         <v>146</v>
       </c>
       <c r="B29" s="4">
@@ -4223,7 +4281,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="16">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="55" t="s">
         <v>147</v>
       </c>
       <c r="B30" s="4">
@@ -4231,7 +4289,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="16">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="55" t="s">
         <v>132</v>
       </c>
       <c r="B31" s="4">
@@ -4239,7 +4297,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="16">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="55" t="s">
         <v>148</v>
       </c>
       <c r="B32" s="4">
@@ -4247,7 +4305,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="16">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="55" t="s">
         <v>149</v>
       </c>
       <c r="B33" s="4">
@@ -4255,7 +4313,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="16">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="55" t="s">
         <v>150</v>
       </c>
       <c r="B34" s="4">
@@ -4297,6 +4355,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4309,8 +4368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4679,7 +4738,7 @@
       <c r="B41" s="37"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="56" t="s">
         <v>192</v>
       </c>
       <c r="B42" s="6"/>

</xml_diff>